<commit_message>
Adding Closeing and enhance
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Studying\Rpa\Session 18\ACME_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA2A2BC-1B1C-4ADA-A96A-989E6F86FFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AEAB05-236D-4898-A5E6-5A6E45002863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,24 @@
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -205,12 +217,6 @@
     <t>Acme Url_WorkItems</t>
   </si>
   <si>
-    <t>retry interval</t>
-  </si>
-  <si>
-    <t>time span+++++</t>
-  </si>
-  <si>
     <t>Retry_Num</t>
   </si>
   <si>
@@ -230,6 +236,30 @@
   </si>
   <si>
     <t>Account value not matches</t>
+  </si>
+  <si>
+    <t>TimeOut_Short</t>
+  </si>
+  <si>
+    <t>TimeOut_Medium</t>
+  </si>
+  <si>
+    <t>TimeOut_Long</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>ControCloseTabs</t>
+  </si>
+  <si>
+    <t>ClientAccountMovemnets,ClientAccounts,ClientDetails,SearchingClient</t>
   </si>
 </sst>
 </file>
@@ -282,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -292,7 +322,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +728,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1711,14 +1755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A5702" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="2" max="2" width="51" style="6" customWidth="1"/>
     <col min="3" max="3" width="75.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -1727,7 +1771,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1761,7 +1805,7 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1772,7 +1816,7 @@
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1784,7 +1828,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -1796,7 +1840,7 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1807,7 +1851,7 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
@@ -1818,7 +1862,7 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
@@ -1829,7 +1873,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
@@ -1840,7 +1884,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
@@ -1851,7 +1895,7 @@
       <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C12" t="s">
@@ -1863,7 +1907,7 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <v>2</v>
       </c>
       <c r="C14" t="s">
@@ -1874,7 +1918,7 @@
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>2</v>
       </c>
       <c r="C15" t="s">
@@ -1886,7 +1930,7 @@
       <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="b">
+      <c r="B17" s="6" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1895,9 +1939,9 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18">
+        <v>60</v>
+      </c>
+      <c r="B18" s="6">
         <v>3</v>
       </c>
     </row>
@@ -1905,7 +1949,7 @@
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1913,7 +1957,7 @@
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1921,7 +1965,7 @@
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1930,48 +1974,85 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>68</v>
-      </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="5">
-        <v>5.7870370370370366E-5</v>
+        <v>61</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="6">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="6">
+        <v>40000</v>
+      </c>
+    </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
+      <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>